<commit_message>
fixed mistake in excel formula for determining quality
</commit_message>
<xml_diff>
--- a/data/score_based_efdata_binary.xlsx
+++ b/data/score_based_efdata_binary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/Machine Learning/ph4_classification/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:40009_{1673F3A0-A6F9-4DED-828E-5A531AA80D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A26F3EF6-5E75-4B89-A1CB-B1097DAAE5D0}"/>
+  <xr:revisionPtr revIDLastSave="166" documentId="13_ncr:40009_{1673F3A0-A6F9-4DED-828E-5A531AA80D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86E4A4DC-4592-46D8-98AF-D4FE49E7C534}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="25420" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="score_based_efdata_binary" sheetId="1" r:id="rId1"/>
@@ -1011,17 +1011,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AC2" sqref="AC2:AC53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1206,11 +1206,11 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <f t="shared" ref="AC2:AC33" si="2">IF(C2&gt;2, 1, 0)</f>
+        <f>IF(D2&gt;2, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -1270,47 +1270,47 @@
         <v>7</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T53" si="3">IF(OR(K3=S3,L3=S3,M3=S3,N3=S3,O3=S3,P3=S3,Q3=S3,R3=S3), 1, 0)</f>
+        <f t="shared" ref="T3:T53" si="2">IF(OR(K3=S3,L3=S3,M3=S3,N3=S3,O3=S3,P3=S3,Q3=S3,R3=S3), 1, 0)</f>
         <v>0</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U34" si="4">K3/$S3</f>
+        <f t="shared" ref="U3:U34" si="3">K3/$S3</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V34" si="5">L3/$S3</f>
+        <f t="shared" ref="V3:V34" si="4">L3/$S3</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W34" si="6">M3/$S3</f>
+        <f t="shared" ref="W3:W34" si="5">M3/$S3</f>
         <v>0</v>
       </c>
       <c r="X3">
-        <f t="shared" ref="X3:X53" si="7">N3/$S3</f>
+        <f t="shared" ref="X3:X53" si="6">N3/$S3</f>
         <v>0</v>
       </c>
       <c r="Y3">
-        <f t="shared" ref="Y3:Y53" si="8">O3/$S3</f>
+        <f t="shared" ref="Y3:Y53" si="7">O3/$S3</f>
         <v>0.42857142857142855</v>
       </c>
       <c r="Z3">
-        <f t="shared" ref="Z3:Z53" si="9">P3/$S3</f>
+        <f t="shared" ref="Z3:Z53" si="8">P3/$S3</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="AA3">
-        <f t="shared" ref="AA3:AA53" si="10">Q3/$S3</f>
+        <f t="shared" ref="AA3:AA53" si="9">Q3/$S3</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f t="shared" ref="AB3:AB53" si="11">R3/$S3</f>
+        <f t="shared" ref="AB3:AB53" si="10">R3/$S3</f>
         <v>0</v>
       </c>
       <c r="AC3">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="AC3:AC53" si="11">IF(D3&gt;2, 1, 0)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1370,47 +1370,47 @@
         <v>7</v>
       </c>
       <c r="T4">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U4">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W4">
+      <c r="X4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z4">
+      <c r="AA4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA4">
+      <c r="AB4">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB4">
+      <c r="AC4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC4">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1470,47 +1470,47 @@
         <v>7</v>
       </c>
       <c r="T5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U5">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U5">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V5">
         <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y5">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z5">
         <f t="shared" si="8"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA5">
+      <c r="AB5">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB5">
+      <c r="AC5">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC5">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -1570,47 +1570,47 @@
         <v>7</v>
       </c>
       <c r="T6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U6">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U6">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V6">
         <f t="shared" si="4"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="V6">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W6">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y6">
+      <c r="Z6">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z6">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA6">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA6">
+        <v>0</v>
+      </c>
+      <c r="AB6">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB6">
+      <c r="AC6">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC6">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1670,47 +1670,47 @@
         <v>7</v>
       </c>
       <c r="T7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U7">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U7">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V7">
         <f t="shared" si="4"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="V7">
+      <c r="W7">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y7">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="Z7">
         <f t="shared" si="8"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="Z7">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA7">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA7">
+        <v>0</v>
+      </c>
+      <c r="AB7">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB7">
+      <c r="AC7">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC7">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1770,47 +1770,47 @@
         <v>7</v>
       </c>
       <c r="T8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U8">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y8">
+      <c r="Z8">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z8">
+      <c r="AA8">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA8">
+      <c r="AB8">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB8">
+      <c r="AC8">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC8">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -1870,47 +1870,47 @@
         <v>7</v>
       </c>
       <c r="T9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U9">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V9">
+      <c r="W9">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W9">
+      <c r="X9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y9">
+        <v>1</v>
+      </c>
+      <c r="Z9">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA9">
+      <c r="AB9">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB9">
+      <c r="AC9">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC9">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1970,47 +1970,47 @@
         <v>7</v>
       </c>
       <c r="T10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U10">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U10">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V10">
         <f t="shared" si="4"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="V10">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="W10">
         <f t="shared" si="5"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="W10">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="X10">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y10">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="Z10">
         <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA10">
+      <c r="AB10">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB10">
+      <c r="AC10">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC10">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -2070,47 +2070,47 @@
         <v>7</v>
       </c>
       <c r="T11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V11">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W11">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y11">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="Z11">
         <f t="shared" si="8"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="Z11">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="AA11">
         <f t="shared" si="9"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="AA11">
+        <v>0</v>
+      </c>
+      <c r="AB11">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB11">
+      <c r="AC11">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC11">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -2170,47 +2170,47 @@
         <v>7</v>
       </c>
       <c r="T12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U12">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V12">
         <f t="shared" si="4"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W12">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="X12">
         <f t="shared" si="6"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y12">
+      <c r="Z12">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z12">
+      <c r="AA12">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA12">
+      <c r="AB12">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB12">
+      <c r="AC12">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC12">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -2270,47 +2270,47 @@
         <v>7</v>
       </c>
       <c r="T13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U13">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V13">
         <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W13">
+      <c r="X13">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y13">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z13">
         <f t="shared" si="8"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA13">
+      <c r="AB13">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB13">
+      <c r="AC13">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC13">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -2370,47 +2370,47 @@
         <v>7</v>
       </c>
       <c r="T14">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U14">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U14">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="V14">
         <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="5"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="V14">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W14">
+      <c r="X14">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="8"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="AB14">
+        <f t="shared" si="10"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="X14">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z14">
-        <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA14">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB14">
+      <c r="AC14">
         <f t="shared" si="11"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="AC14">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -2470,47 +2470,47 @@
         <v>7</v>
       </c>
       <c r="T15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U15">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U15">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V15">
         <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W15">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="X15">
         <f t="shared" si="6"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y15">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="Z15">
         <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="Z15">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="AA15">
         <f t="shared" si="9"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="AA15">
+        <v>0</v>
+      </c>
+      <c r="AB15">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB15">
+      <c r="AC15">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -2570,47 +2570,47 @@
         <v>7</v>
       </c>
       <c r="T16">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U16">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U16">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="V16">
         <f t="shared" si="4"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y16">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="Z16">
         <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA16">
+      <c r="AB16">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB16">
+      <c r="AC16">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC16">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -2670,47 +2670,47 @@
         <v>7</v>
       </c>
       <c r="T17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U17">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V17">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W17">
         <f t="shared" si="5"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y17">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="Z17">
         <f t="shared" si="8"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA17">
+      <c r="AB17">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB17">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="AC17">
         <f t="shared" si="11"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="AC17">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -2770,47 +2770,47 @@
         <v>7</v>
       </c>
       <c r="T18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U18">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U18">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V18">
         <f t="shared" si="4"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V18">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W18">
         <f t="shared" si="5"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y18">
+      <c r="Z18">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z18">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA18">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB18">
+      <c r="AC18">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC18">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -2870,47 +2870,47 @@
         <v>7</v>
       </c>
       <c r="T19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U19">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U19">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V19">
         <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y19">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="Z19">
         <f t="shared" si="8"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA19">
+      <c r="AB19">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB19">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AC19">
         <f t="shared" si="11"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AC19">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -2970,47 +2970,47 @@
         <v>7</v>
       </c>
       <c r="T20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U20">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U20">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="V20">
         <f t="shared" si="4"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y20">
+      <c r="Z20">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z20">
+      <c r="AA20">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA20">
+      <c r="AB20">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB20">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AC20">
         <f t="shared" si="11"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AC20">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>34</v>
       </c>
@@ -3070,47 +3070,47 @@
         <v>7</v>
       </c>
       <c r="T21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U21">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y21">
+        <v>1</v>
+      </c>
+      <c r="Z21">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA21">
+      <c r="AB21">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB21">
+      <c r="AC21">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC21">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>35</v>
       </c>
@@ -3170,47 +3170,47 @@
         <v>7</v>
       </c>
       <c r="T22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U22">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U22">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V22">
         <f t="shared" si="4"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="V22">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W22">
         <f t="shared" si="5"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y22">
+      <c r="Z22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z22">
+      <c r="AA22">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA22">
+      <c r="AB22">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB22">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="AC22">
         <f t="shared" si="11"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="AC22">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -3270,47 +3270,47 @@
         <v>7</v>
       </c>
       <c r="T23">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U23">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V23">
+      <c r="W23">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W23">
+      <c r="X23">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X23">
+      <c r="Y23">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y23">
+        <v>1</v>
+      </c>
+      <c r="Z23">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA23">
+      <c r="AB23">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB23">
+      <c r="AC23">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC23">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>35</v>
       </c>
@@ -3370,47 +3370,47 @@
         <v>7</v>
       </c>
       <c r="T24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U24">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U24">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="V24">
         <f t="shared" si="4"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="V24">
+      <c r="W24">
         <f t="shared" si="5"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="W24">
+      <c r="X24">
         <f t="shared" si="6"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y24">
+      <c r="Z24">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z24">
+      <c r="AA24">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA24">
+      <c r="AB24">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB24">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AC24">
         <f t="shared" si="11"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AC24">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -3470,47 +3470,47 @@
         <v>7</v>
       </c>
       <c r="T25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U25">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V25">
+      <c r="W25">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W25">
+      <c r="X25">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X25">
+      <c r="Y25">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y25">
+        <v>1</v>
+      </c>
+      <c r="Z25">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA25">
+      <c r="AB25">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB25">
+      <c r="AC25">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC25">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -3570,47 +3570,47 @@
         <v>7</v>
       </c>
       <c r="T26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U26">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U26">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V26">
         <f t="shared" si="4"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="V26">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W26">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X26">
+      <c r="Y26">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y26">
+      <c r="Z26">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z26">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA26">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA26">
+        <v>0</v>
+      </c>
+      <c r="AB26">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB26">
+      <c r="AC26">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC26">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -3670,47 +3670,47 @@
         <v>7</v>
       </c>
       <c r="T27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U27">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V27">
+      <c r="W27">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W27">
+      <c r="X27">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X27">
+      <c r="Y27">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y27">
+        <v>1</v>
+      </c>
+      <c r="Z27">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA27">
+      <c r="AB27">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB27">
+      <c r="AC27">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC27">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -3770,47 +3770,47 @@
         <v>7</v>
       </c>
       <c r="T28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U28">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U28">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V28">
         <f t="shared" si="4"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V28">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="W28">
         <f t="shared" si="5"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="W28">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="X28">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X28">
+        <v>0</v>
+      </c>
+      <c r="Y28">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y28">
+      <c r="Z28">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z28">
+      <c r="AA28">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA28">
+      <c r="AB28">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB28">
+      <c r="AC28">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC28">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -3870,47 +3870,47 @@
         <v>7</v>
       </c>
       <c r="T29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U29">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U29">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V29">
         <f t="shared" si="4"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V29">
+        <v>0</v>
+      </c>
+      <c r="W29">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X29">
+      <c r="Y29">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y29">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z29">
         <f t="shared" si="8"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA29">
+      <c r="AB29">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB29">
+      <c r="AC29">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC29">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
@@ -3970,47 +3970,47 @@
         <v>7</v>
       </c>
       <c r="T30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U30">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U30">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V30">
         <f t="shared" si="4"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="V30">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W30">
         <f t="shared" si="5"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W30">
+      <c r="X30">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X30">
+        <v>0</v>
+      </c>
+      <c r="Y30">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y30">
+      <c r="Z30">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z30">
+      <c r="AA30">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA30">
+      <c r="AB30">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB30">
+      <c r="AC30">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC30">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -4070,47 +4070,47 @@
         <v>7</v>
       </c>
       <c r="T31">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U31">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U31">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V31">
         <f t="shared" si="4"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="V31">
+      <c r="W31">
         <f t="shared" si="5"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W31">
+        <v>0</v>
+      </c>
+      <c r="X31">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X31">
+      <c r="Y31">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y31">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="Z31">
         <f t="shared" si="8"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="Z31">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA31">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA31">
+        <v>0</v>
+      </c>
+      <c r="AB31">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB31">
+      <c r="AC31">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC31">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -4170,47 +4170,47 @@
         <v>7</v>
       </c>
       <c r="T32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U32">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="U32">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="V32">
         <f t="shared" si="4"/>
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="W32">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="X32">
         <f t="shared" si="6"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y32">
+      <c r="Z32">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z32">
+      <c r="AA32">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA32">
+      <c r="AB32">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB32">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AC32">
         <f t="shared" si="11"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AC32">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -4270,47 +4270,47 @@
         <v>7</v>
       </c>
       <c r="T33">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="U33">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="U33">
+        <v>0</v>
+      </c>
+      <c r="V33">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="V33">
+      <c r="W33">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="X33">
+      <c r="Y33">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y33">
+        <v>1</v>
+      </c>
+      <c r="Z33">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA33">
+      <c r="AB33">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB33">
+      <c r="AC33">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC33">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -4370,47 +4370,47 @@
         <v>7</v>
       </c>
       <c r="T34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="U34">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="U34">
+      <c r="V34">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="V34">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="W34">
         <f t="shared" si="5"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="W34">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="X34">
         <f t="shared" si="6"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="X34">
+        <v>0</v>
+      </c>
+      <c r="Y34">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y34">
+      <c r="Z34">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z34">
+      <c r="AA34">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA34">
+      <c r="AB34">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB34">
+      <c r="AC34">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC34">
-        <f t="shared" ref="AC34:AC53" si="12">IF(C34&gt;2, 1, 0)</f>
-        <v>1</v>
-      </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>38</v>
       </c>
@@ -4470,47 +4470,47 @@
         <v>7</v>
       </c>
       <c r="T35">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U35">
-        <f t="shared" ref="U35:U53" si="13">K35/$S35</f>
+        <f t="shared" ref="U35:U53" si="12">K35/$S35</f>
         <v>0</v>
       </c>
       <c r="V35">
-        <f t="shared" ref="V35:V53" si="14">L35/$S35</f>
+        <f t="shared" ref="V35:V53" si="13">L35/$S35</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="W35">
-        <f t="shared" ref="W35:W53" si="15">M35/$S35</f>
+        <f t="shared" ref="W35:W53" si="14">M35/$S35</f>
         <v>0.14285714285714285</v>
       </c>
       <c r="X35">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y35">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y35">
+      <c r="Z35">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z35">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="AA35">
         <f t="shared" si="9"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="AA35">
+        <v>0</v>
+      </c>
+      <c r="AB35">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB35">
+      <c r="AC35">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC35">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -4570,47 +4570,47 @@
         <v>7</v>
       </c>
       <c r="T36">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U36">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="V36">
         <f t="shared" si="13"/>
-        <v>1</v>
-      </c>
-      <c r="V36">
+        <v>0</v>
+      </c>
+      <c r="W36">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W36">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X36">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y36">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y36">
+      <c r="Z36">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z36">
+      <c r="AA36">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA36">
+      <c r="AB36">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB36">
+      <c r="AC36">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC36">
-        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -4670,47 +4670,47 @@
         <v>7</v>
       </c>
       <c r="T37">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U37">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="V37">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="V37">
+      <c r="W37">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W37">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X37">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y37">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y37">
+        <v>1</v>
+      </c>
+      <c r="Z37">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA37">
+      <c r="AB37">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB37">
+      <c r="AC37">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC37">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -4770,47 +4770,47 @@
         <v>7</v>
       </c>
       <c r="T38">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U38">
+        <f t="shared" si="12"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="V38">
         <f t="shared" si="13"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="V38">
+        <v>0</v>
+      </c>
+      <c r="W38">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W38">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X38">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y38">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y38">
+      <c r="Z38">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z38">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA38">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA38">
+        <v>0</v>
+      </c>
+      <c r="AB38">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB38">
+      <c r="AC38">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC38">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -4870,47 +4870,47 @@
         <v>7</v>
       </c>
       <c r="T39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U39">
+        <f t="shared" si="12"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="V39">
         <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="W39">
+        <f t="shared" si="14"/>
         <v>0.2857142857142857</v>
       </c>
-      <c r="V39">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="W39">
-        <f t="shared" si="15"/>
-        <v>0.2857142857142857</v>
-      </c>
       <c r="X39">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y39">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y39">
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="Z39">
         <f t="shared" si="8"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA39">
+      <c r="AB39">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB39">
+      <c r="AC39">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC39">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -4970,47 +4970,47 @@
         <v>7</v>
       </c>
       <c r="T40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U40">
+        <f t="shared" si="12"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V40">
         <f t="shared" si="13"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V40">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W40">
         <f t="shared" si="14"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W40">
-        <f t="shared" si="15"/>
-        <v>0.14285714285714285</v>
-      </c>
       <c r="X40">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y40">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y40">
+      <c r="Z40">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z40">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA40">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA40">
+        <v>0</v>
+      </c>
+      <c r="AB40">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB40">
+      <c r="AC40">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC40">
-        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -5070,47 +5070,47 @@
         <v>7</v>
       </c>
       <c r="T41">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="U41">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="V41">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="V41">
+      <c r="W41">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W41">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X41">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y41">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y41">
+        <v>1</v>
+      </c>
+      <c r="Z41">
         <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-      <c r="Z41">
+        <v>0</v>
+      </c>
+      <c r="AA41">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA41">
+      <c r="AB41">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB41">
+      <c r="AC41">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC41">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -5170,47 +5170,47 @@
         <v>7</v>
       </c>
       <c r="T42">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U42">
+        <f t="shared" si="12"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V42">
         <f t="shared" si="13"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V42">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W42">
         <f t="shared" si="14"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W42">
-        <f t="shared" si="15"/>
-        <v>0.14285714285714285</v>
-      </c>
       <c r="X42">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y42">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y42">
+      <c r="Z42">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="Z42">
+      <c r="AA42">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA42">
+      <c r="AB42">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB42">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AC42">
         <f t="shared" si="11"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AC42">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -5270,47 +5270,47 @@
         <v>7</v>
       </c>
       <c r="T43">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U43">
+        <f t="shared" si="12"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V43">
         <f t="shared" si="13"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="V43">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W43">
         <f t="shared" si="14"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W43">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X43">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y43">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y43">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="Z43">
         <f t="shared" si="8"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="Z43">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA43">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA43">
+        <v>0</v>
+      </c>
+      <c r="AB43">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB43">
+      <c r="AC43">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC43">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -5370,47 +5370,47 @@
         <v>7</v>
       </c>
       <c r="T44">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U44">
+        <f t="shared" si="12"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V44">
         <f t="shared" si="13"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="V44">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W44">
         <f t="shared" si="14"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W44">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X44">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y44">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y44">
+      <c r="Z44">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z44">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA44">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA44">
+        <v>0</v>
+      </c>
+      <c r="AB44">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB44">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="AC44">
         <f t="shared" si="11"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="AC44">
-        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>40</v>
       </c>
@@ -5470,47 +5470,47 @@
         <v>7</v>
       </c>
       <c r="T45">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U45">
+        <f t="shared" si="12"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V45">
         <f t="shared" si="13"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W45">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X45">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y45">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y45">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="Z45">
         <f t="shared" si="8"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA45">
+      <c r="AB45">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB45">
+      <c r="AC45">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC45">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>41</v>
       </c>
@@ -5570,47 +5570,47 @@
         <v>7</v>
       </c>
       <c r="T46">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U46">
+        <f t="shared" si="12"/>
+        <v>0.42857142857142855</v>
+      </c>
+      <c r="V46">
         <f t="shared" si="13"/>
-        <v>0.42857142857142855</v>
-      </c>
-      <c r="V46">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="W46">
         <f t="shared" si="14"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="W46">
-        <f t="shared" si="15"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="X46">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y46">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y46">
+      <c r="Z46">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z46">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA46">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AB46">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB46">
+      <c r="AC46">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC46">
-        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>41</v>
       </c>
@@ -5670,47 +5670,47 @@
         <v>7</v>
       </c>
       <c r="T47">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U47">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="V47">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="V47">
+      <c r="W47">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="W47">
-        <f t="shared" si="15"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="X47">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y47">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y47">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z47">
         <f t="shared" si="8"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA47">
+      <c r="AB47">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB47">
+      <c r="AC47">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-      <c r="AC47">
-        <f t="shared" si="12"/>
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -5770,47 +5770,47 @@
         <v>7</v>
       </c>
       <c r="T48">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U48">
+        <f t="shared" si="12"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V48">
         <f t="shared" si="13"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V48">
+        <v>0</v>
+      </c>
+      <c r="W48">
         <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="W48">
-        <f t="shared" si="15"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="X48">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y48">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y48">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="Z48">
         <f t="shared" si="8"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA48">
+      <c r="AB48">
         <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="AB48">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AC48">
         <f t="shared" si="11"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AC48">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>41</v>
       </c>
@@ -5870,47 +5870,47 @@
         <v>7</v>
       </c>
       <c r="T49">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U49">
+        <f t="shared" si="12"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V49">
         <f t="shared" si="13"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W49">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X49">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y49">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y49">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z49">
         <f t="shared" si="8"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="Z49">
+        <v>0</v>
+      </c>
+      <c r="AA49">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA49">
+      <c r="AB49">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB49">
+      <c r="AC49">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC49">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>42</v>
       </c>
@@ -5970,47 +5970,47 @@
         <v>7</v>
       </c>
       <c r="T50">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U50">
+        <f t="shared" si="12"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V50">
         <f t="shared" si="13"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V50">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W50">
         <f t="shared" si="14"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W50">
-        <f t="shared" si="15"/>
-        <v>0.14285714285714285</v>
-      </c>
       <c r="X50">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y50">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y50">
+      <c r="Z50">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z50">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA50">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA50">
+        <v>0</v>
+      </c>
+      <c r="AB50">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB50">
+      <c r="AC50">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC50">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -6070,47 +6070,47 @@
         <v>7</v>
       </c>
       <c r="T51">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U51">
+        <f t="shared" si="12"/>
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="V51">
         <f t="shared" si="13"/>
-        <v>0.2857142857142857</v>
-      </c>
-      <c r="V51">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W51">
         <f t="shared" si="14"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="W51">
-        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="X51">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y51">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y51">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="Z51">
         <f t="shared" si="8"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="Z51">
+        <v>0</v>
+      </c>
+      <c r="AA51">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA51">
+      <c r="AB51">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB51">
+      <c r="AC51">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC51">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>42</v>
       </c>
@@ -6170,47 +6170,47 @@
         <v>7</v>
       </c>
       <c r="T52">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U52">
+        <f t="shared" si="12"/>
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="V52">
         <f t="shared" si="13"/>
-        <v>0.5714285714285714</v>
-      </c>
-      <c r="V52">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="W52">
         <f t="shared" si="14"/>
         <v>0.14285714285714285</v>
       </c>
-      <c r="W52">
-        <f t="shared" si="15"/>
-        <v>0.14285714285714285</v>
-      </c>
       <c r="X52">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y52">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y52">
+      <c r="Z52">
         <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="Z52">
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="AA52">
         <f t="shared" si="9"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="AA52">
+        <v>0</v>
+      </c>
+      <c r="AB52">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB52">
+      <c r="AC52">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AC52">
-        <f t="shared" si="12"/>
-        <v>1</v>
-      </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>42</v>
       </c>
@@ -6270,44 +6270,44 @@
         <v>7</v>
       </c>
       <c r="T53">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="U53">
+        <f t="shared" si="12"/>
+        <v>0.14285714285714285</v>
+      </c>
+      <c r="V53">
         <f t="shared" si="13"/>
-        <v>0.14285714285714285</v>
-      </c>
-      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
         <f t="shared" si="14"/>
         <v>0</v>
       </c>
-      <c r="W53">
-        <f t="shared" si="15"/>
-        <v>0</v>
-      </c>
       <c r="X53">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y53">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="Y53">
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="Z53">
         <f t="shared" si="8"/>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="Z53">
+        <v>0</v>
+      </c>
+      <c r="AA53">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AA53">
+      <c r="AB53">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="AB53">
+      <c r="AC53">
         <f t="shared" si="11"/>
         <v>0</v>
-      </c>
-      <c r="AC53">
-        <f t="shared" si="12"/>
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>